<commit_message>
add final energy consumption calculation module in excel file
</commit_message>
<xml_diff>
--- a/xlsx/data.xlsx
+++ b/xlsx/data.xlsx
@@ -13,13 +13,18 @@
     <sheet name="iTRA" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="iCOM" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="iRES" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="sIND" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="LOSS" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="sIND" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="sTRA" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="sCOM" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="sRES" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="sELE" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -51,6 +56,9 @@
     <t xml:space="preserve">Residential</t>
   </si>
   <si>
+    <t xml:space="preserve">ELE</t>
+  </si>
+  <si>
     <t xml:space="preserve">COL</t>
   </si>
   <si>
@@ -63,7 +71,31 @@
     <t xml:space="preserve">BMS</t>
   </si>
   <si>
-    <t xml:space="preserve">ELE</t>
+    <t xml:space="preserve">COLX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OILX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GASX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMSX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HYD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PV</t>
   </si>
 </sst>
 </file>
@@ -737,6 +769,1418 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0000127563610961359</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.976242188627097</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.00127593983249683</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.00252089993090304</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0199482152484074</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0000130761890381062</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.97628601984156</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.00128582525541378</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.00251280766015607</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0199022710538319</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0000122700235773222</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.976158085725306</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.00122448542981893</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.00258677266289086</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0200183861584066</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0000120951891385202</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.97548941750524</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.00113121847890265</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.00306135602984965</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0203059127968693</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2014</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0000124358001815627</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.974323345204068</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.00109827751077169</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.00382662661902664</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0207393148659519</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2015</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0000121347680783447</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.97356260392445</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.000978980613888078</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.00472436038293392</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0207219203106501</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0000132625027271021</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.972840052227736</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.000840511110330097</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.00536667172852187</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0209395024306852</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0000133731630706788</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.972273086676485</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.000719476173202521</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.00587984547310072</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0211142185141413</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2018</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0000121864816036597</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.972229378018905</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.000593752464800533</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.00607733067306953</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0210873523616217</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2019</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0000124402436352604</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.972049191487832</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.000483441690159145</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.00592846721684796</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0215264593615252</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0000137654722952663</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.968745495153598</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.000406463806940781</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.00701465525712946</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0238196203100367</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.00465182109398443</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.248780292784875</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.163919367208958</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.025323313743574</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.557325205168608</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.00443937837618143</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.247661613325155</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.170166010212602</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0269752739741212</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.55075772411194</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.00370231464474871</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.241225779086881</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.168257442302387</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.028215585444752</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.558598878521231</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.00377392792263585</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.267811848087296</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.166527881251453</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0293294768802379</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.532556865858377</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2014</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0036354345163539</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.255314983044822</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.167067980866524</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0296629979050195</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.54431860366728</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2015</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.00384221225809996</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.235266941064898</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.186677432377876</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.030863828882524</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.543349585416602</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.00344430509299673</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.22954751401036</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.172581337311204</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0318521241103312</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.562574719475109</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.00352644182596447</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.216322072075319</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.186930731705442</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0336621891716418</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.559558565221633</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2018</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.00227920610692883</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.240628984112254</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.176965719300653</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0340575770647568</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.546068513415407</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2019</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.00254169586888653</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.215081088233997</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.188233506667908</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0355763905566147</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.558567318672594</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.00269743384889377</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.235100657037878</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.155260048019108</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.0375768243307909</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.569365036763329</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.295577388456578</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.185649697865496</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.000194660599825144</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.518578253078101</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.294781866130855</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.192891623759889</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.000179329398467914</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.512147180710787</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.292714418499285</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.190718860799803</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.000168908764924207</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.516397811935988</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.288747412097999</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.191014059935836</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.000173333992682247</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.520065193973483</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2014</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.282634731811053</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.199357563841297</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.000180578946725493</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.517827125400925</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2015</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.276882966712301</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.196515236635559</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.000185446790406947</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.526416349861733</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.275029440633412</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.200188136813701</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.00018519547382262</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.524597227079064</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.282907320193399</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.201477249685925</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.000177679670728215</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.515437750449948</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2018</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.261349883050479</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.204412917935886</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.000192649405279954</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.534044549608355</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2019</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.272207345338359</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.208935466078323</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.000194336241708559</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.518662852341609</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.267849508803155</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.212616037620618</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.00018539845399501</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.519349055122232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.277508981658784</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0794383653074846</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.290670709251437</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.252133772699081</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.0180280502430537</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.0733053816472367</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.00230238382452896</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.00351305981736638</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.00309929555102816</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.279514031567449</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.138739425883535</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.378150073272013</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.093966393678015</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.0199593518081612</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.0784135200946303</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.00247102592822759</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.00431783155470561</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.00446834621326357</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.309036885418116</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.16871896917671</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.401733664142025</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.0148835897660963</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.0210362952663667</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.0714615873774758</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.00243624353471017</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.00451764899230655</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.00617511632619331</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.32857950846392</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.137454759567475</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.410167848157459</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0086399126257143</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.0222308490295306</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.0737313407885046</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.00241746668437432</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.00481728762652694</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.0119610270564952</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.334326080980433</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.101734914500362</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.431595057885971</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.0236005064249575</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.0794565919426686</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.00249217390808064</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.00496246995360942</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.0218322044039186</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.341673503664889</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0884855919937461</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.410509175767614</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.00913029512612327</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.0243335861732676</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.0842866430854728</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.00251066184722792</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.00539864859635136</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.0336718937453076</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.330675581183728</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0705485684728781</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.420809586298719</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.0172990162741022</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0323968620389084</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.0761357867412523</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.00239561681625303</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.00590618684087012</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.0438327953332886</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.331369893457585</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0577521051101989</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.403932324957214</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.0312580134749847</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0353048777013127</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.0795838976402631</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.00233352391553346</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.00616384624005379</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.052301517502854</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.319154245328742</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0437033390053524</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.389648517165296</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.0623144717104449</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.0377251652419438</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.0777076213317824</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.00242236483847222</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.00717975885761121</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.0601445165203554</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.322438841124481</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0343351533002472</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.381051176338918</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.0628909173560157</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.0416705698826866</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.0788791475573428</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.00280735730746134</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.00751093804388234</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.0684158990889647</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.313426983789406</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0321379578663662</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.397941195147002</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.0390594368272674</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.0462308832823151</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.0794322109322477</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.00301573686486334</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.00904116299392519</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.0797144322966066</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
@@ -2031,25 +3475,135 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.905095428809249</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.906341796876974</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.90931390033079</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.905790118440597</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.910844163083025</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.911547003404931</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.897322110943927</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.899794083235142</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.8983272718829</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.898813117102369</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.89526829442089</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
modify blast furnace value and add data output script
</commit_message>
<xml_diff>
--- a/xlsx/data.xlsx
+++ b/xlsx/data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t xml:space="preserve">EMI_LULUCF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blast furnaces</t>
   </si>
 </sst>
 </file>
@@ -1661,530 +1658,1037 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="n">
         <v>2010</v>
       </c>
-      <c r="B2" t="n">
-        <v>0.277508981658784</v>
-      </c>
       <c r="C2" t="n">
+        <v>0.235317279731797</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.2542029283506</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.118208827636883</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0364559087844255</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.355815055496294</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.233781164697422</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.265632827450878</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.123996041168318</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0393771825968263</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.337212784086556</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.238183139592608</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.254729802181916</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.126204574849316</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0385824030204225</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.342300080355736</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.238991514104705</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.25628028219994</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.118880058675235</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0418285950752597</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.34401954994486</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2014</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.239516304821693</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.252808385648269</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.119951336210655</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0394015934257564</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.348322379893626</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2015</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.244278082479678</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.240704426350651</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.123588729268783</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.040869790218956</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.350558971681932</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.242373154334521</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.228317868362445</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.130553448532646</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0424868181183189</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.356268710652069</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.24922368028528</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.217978539482308</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.130354331207477</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0435277511261819</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.358915697898754</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2018</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.242436419524306</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.217749202182963</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.136550016297178</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0452056222686474</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.358058739726906</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2019</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.246172595109221</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.21124427442343</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.134886409911155</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0459790921710079</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.361717628385187</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.2378380422764</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.218958939914931</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.134617175435078</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.0445472571891143</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.364038585184477</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0000127563610961359</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.976242188627097</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.00127593983249683</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.00252089993090304</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0199482152484074</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0000130761890381062</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.97628601984156</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.00128582525541378</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.00251280766015607</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0199022710538319</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0000122700235773222</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.976158085725306</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.00122448542981893</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.00258677266289086</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.0200183861584066</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0000120951891385202</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.97548941750524</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.00113121847890265</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.00306135602984965</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.0203059127968693</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2014</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0000124358001815627</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.974323345204068</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.00109827751077169</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.00382662661902664</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.0207393148659519</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2015</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0000121347680783447</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.97356260392445</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.000978980613888078</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.00472436038293392</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.0207219203106501</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0000132625027271021</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.972840052227736</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.000840511110330097</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.00536667172852187</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.0209395024306852</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0000133731630706788</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.972273086676485</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.000719476173202521</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.00587984547310072</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.0211142185141413</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2018</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0000121864816036597</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.972229378018905</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.000593752464800533</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.00607733067306953</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.0210873523616217</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="n">
+        <v>2019</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0000124402436352604</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.972049191487832</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.000483441690159145</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.00592846721684796</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.0215264593615252</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0000137654722952663</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.968745495153598</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.000406463806940781</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.00701465525712946</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.0238196203100367</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C24" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
-        <v>0.0794383653074846</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="D24" t="n">
+        <v>0.295577388456578</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.185649697865496</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.000194660599825144</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.518578253078101</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C25" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="n">
-        <v>0.290670709251437</v>
-      </c>
-      <c r="G2" t="n">
+      <c r="D25" t="n">
+        <v>0.294781866130855</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.192891623759889</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.000179329398467914</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.512147180710787</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C26" t="n">
         <v>0</v>
       </c>
-      <c r="H2" t="n">
-        <v>0.252133772699081</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.0180280502430537</v>
-      </c>
-      <c r="J2" t="n">
+      <c r="D26" t="n">
+        <v>0.292714418499285</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.190718860799803</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.000168908764924207</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.516397811935988</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C27" t="n">
         <v>0</v>
       </c>
-      <c r="K2" t="n">
-        <v>0.0733053816472367</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.00230238382452896</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.00351305981736638</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.00309929555102816</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
+      <c r="D27" t="n">
+        <v>0.288747412097999</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.191014059935836</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.000173333992682247</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.520065193973483</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2014</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.282634731811053</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.199357563841297</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.000180578946725493</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.517827125400925</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" t="n">
+        <v>2015</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.276882966712301</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.196515236635559</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.000185446790406947</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.526416349861733</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.275029440633412</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.200188136813701</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.00018519547382262</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.524597227079064</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.282907320193399</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.201477249685925</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.000177679670728215</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.515437750449948</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" t="n">
+        <v>2018</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.261349883050479</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.204412917935886</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.000192649405279954</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.534044549608355</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" t="n">
+        <v>2019</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.272207345338359</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.208935466078323</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.000194336241708559</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.518662852341609</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.267849508803155</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.212616037620618</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.00018539845399501</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.519349055122232</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.00465182109398443</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.248780292784875</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.163919367208958</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.025323313743574</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.557325205168608</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" t="n">
         <v>2011</v>
       </c>
-      <c r="B3" t="n">
-        <v>0.279514031567449</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.138739425883535</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.378150073272013</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.093966393678015</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.0199593518081612</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.0784135200946303</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.00247102592822759</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.00431783155470561</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.00446834621326357</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
+      <c r="C36" t="n">
+        <v>0.00443937837618143</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.247661613325155</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.170166010212602</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.0269752739741212</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.55075772411194</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="n">
         <v>2012</v>
       </c>
-      <c r="B4" t="n">
-        <v>0.309036885418116</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.16871896917671</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.401733664142025</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.0148835897660963</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.0210362952663667</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.0714615873774758</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.00243624353471017</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.00451764899230655</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.00617511632619331</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
+      <c r="C37" t="n">
+        <v>0.00370231464474871</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.241225779086881</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.168257442302387</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.028215585444752</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.558598878521231</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" t="n">
         <v>2013</v>
       </c>
-      <c r="B5" t="n">
-        <v>0.32857950846392</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.137454759567475</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.410167848157459</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.0086399126257143</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.0222308490295306</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.0737313407885046</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.00241746668437432</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.00481728762652694</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.0119610270564952</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
+      <c r="C38" t="n">
+        <v>0.00377392792263585</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.267811848087296</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.166527881251453</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.0293294768802379</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.532556865858377</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="n">
         <v>2014</v>
       </c>
-      <c r="B6" t="n">
-        <v>0.334326080980433</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.101734914500362</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.431595057885971</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.0236005064249575</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.0794565919426686</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.00249217390808064</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.00496246995360942</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.0218322044039186</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
+      <c r="C39" t="n">
+        <v>0.0036354345163539</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.255314983044822</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.167067980866524</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.0296629979050195</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.54431860366728</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="n">
         <v>2015</v>
       </c>
-      <c r="B7" t="n">
-        <v>0.341673503664889</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.0884855919937461</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.410509175767614</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.00913029512612327</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.0243335861732676</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.0842866430854728</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.00251066184722792</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.00539864859635136</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.0336718937453076</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
+      <c r="C40" t="n">
+        <v>0.00384221225809996</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.235266941064898</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.186677432377876</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.030863828882524</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.543349585416602</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="n">
         <v>2016</v>
       </c>
-      <c r="B8" t="n">
-        <v>0.330675581183728</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.0705485684728781</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.420809586298719</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.0172990162741022</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.0323968620389084</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.0761357867412523</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.00239561681625303</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.00590618684087012</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.0438327953332886</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
+      <c r="C41" t="n">
+        <v>0.00344430509299673</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.22954751401036</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.172581337311204</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.0318521241103312</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.562574719475109</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" t="n">
         <v>2017</v>
       </c>
-      <c r="B9" t="n">
-        <v>0.331369893457585</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.0577521051101989</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.403932324957214</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.0312580134749847</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.0353048777013127</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.0795838976402631</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.00233352391553346</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.00616384624005379</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0.052301517502854</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
+      <c r="C42" t="n">
+        <v>0.00352644182596447</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.216322072075319</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.186930731705442</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.0336621891716418</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.559558565221633</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" t="n">
         <v>2018</v>
       </c>
-      <c r="B10" t="n">
-        <v>0.319154245328742</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.0437033390053524</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.389648517165296</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.0623144717104449</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.0377251652419438</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.0777076213317824</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.00242236483847222</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.00717975885761121</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0.0601445165203554</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
+      <c r="C43" t="n">
+        <v>0.00227920610692883</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.240628984112254</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.176965719300653</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.0340575770647568</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.546068513415407</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" t="n">
         <v>2019</v>
       </c>
-      <c r="B11" t="n">
-        <v>0.322438841124481</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.0343351533002472</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.381051176338918</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.0628909173560157</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.0416705698826866</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.0788791475573428</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.00280735730746134</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0.00751093804388234</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0.0684158990889647</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
+      <c r="C44" t="n">
+        <v>0.00254169586888653</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.215081088233997</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.188233506667908</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.0355763905566147</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.558567318672594</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="n">
         <v>2020</v>
       </c>
-      <c r="B12" t="n">
-        <v>0.313426983789406</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.0321379578663662</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.397941195147002</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.0390594368272674</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0.0462308832823151</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.0794322109322477</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.00301573686486334</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0.00904116299392519</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.0797144322966066</v>
+      <c r="C45" t="n">
+        <v>0.00269743384889377</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.235100657037878</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.155260048019108</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.0375768243307909</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.569365036763329</v>
       </c>
     </row>
   </sheetData>
@@ -4723,134 +5227,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>25</v>
+      <c r="A2" t="n">
+        <v>2010</v>
       </c>
       <c r="B2" t="n">
-        <v>2010</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.136976765300607</v>
+        <v>0.154347028848067</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>25</v>
+      <c r="A3" t="n">
+        <v>2011</v>
       </c>
       <c r="B3" t="n">
-        <v>2011</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.128498162479982</v>
+        <v>0.144116657652733</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>25</v>
+      <c r="A4" t="n">
+        <v>2012</v>
       </c>
       <c r="B4" t="n">
-        <v>2012</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.131182868197745</v>
+        <v>0.145612538466151</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>25</v>
+      <c r="A5" t="n">
+        <v>2013</v>
       </c>
       <c r="B5" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.135989996396184</v>
+        <v>0.151571753065132</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>25</v>
+      <c r="A6" t="n">
+        <v>2014</v>
       </c>
       <c r="B6" t="n">
-        <v>2014</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.133695870123065</v>
+        <v>0.14932172493144</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>25</v>
+      <c r="A7" t="n">
+        <v>2015</v>
       </c>
       <c r="B7" t="n">
-        <v>2015</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.125863777485224</v>
+        <v>0.140708085157738</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>25</v>
+      <c r="A8" t="n">
+        <v>2016</v>
       </c>
       <c r="B8" t="n">
-        <v>2016</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.124347028156709</v>
+        <v>0.139336403700608</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>25</v>
+      <c r="A9" t="n">
+        <v>2017</v>
       </c>
       <c r="B9" t="n">
-        <v>2017</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.119926602421328</v>
+        <v>0.134461525118918</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>25</v>
+      <c r="A10" t="n">
+        <v>2018</v>
       </c>
       <c r="B10" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.116891761105658</v>
+        <v>0.132622725426858</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>25</v>
+      <c r="A11" t="n">
+        <v>2019</v>
       </c>
       <c r="B11" t="n">
-        <v>2019</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.112810484717389</v>
+        <v>0.127302557927408</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>25</v>
+      <c r="A12" t="n">
+        <v>2020</v>
       </c>
       <c r="B12" t="n">
-        <v>2020</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.0901562318835952</v>
+        <v>0.102806674705956</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add LCOE and import dependency calculation module and prototype of household expenditure calculation.
</commit_message>
<xml_diff>
--- a/xlsx/data.xlsx
+++ b/xlsx/data.xlsx
@@ -25,12 +25,14 @@
     <sheet name="EMI_WASTE" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="EMI_LULUCF" sheetId="18" state="visible" r:id="rId18"/>
     <sheet name="IND_BF" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="LCOE" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="EPT" sheetId="21" state="visible" r:id="rId21"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -77,6 +79,30 @@
     <t xml:space="preserve">BMS</t>
   </si>
   <si>
+    <t xml:space="preserve">PRM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHR_SEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HYD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WIN</t>
+  </si>
+  <si>
     <t xml:space="preserve">COLX</t>
   </si>
   <si>
@@ -86,25 +112,13 @@
     <t xml:space="preserve">GASX</t>
   </si>
   <si>
-    <t xml:space="preserve">NUC</t>
-  </si>
-  <si>
     <t xml:space="preserve">BMSX</t>
   </si>
   <si>
-    <t xml:space="preserve">HYD</t>
+    <t xml:space="preserve">EMI_LULUCF</t>
   </si>
   <si>
-    <t xml:space="preserve">GEO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMI_LULUCF</t>
+    <t xml:space="preserve">value</t>
   </si>
 </sst>
 </file>
@@ -1661,527 +1675,2631 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
         <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>2010</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="n">
         <v>0.277508981658784</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.0794383653074846</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.290670709251437</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.252133772699081</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.0180280502430537</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.0733053816472367</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.00230238382452896</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.00351305981736638</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.00309929555102816</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2011</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.279514031567449</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
+        <v>2010</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>0.138739425883535</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.378150073272013</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.093966393678015</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.0199593518081612</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.0784135200946303</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.00247102592822759</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.00431783155470561</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.00446834621326357</v>
+        <v>0.0794383653074846</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2012</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.309036885418116</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
+        <v>2010</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>0.16871896917671</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.401733664142025</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.0148835897660963</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.0210362952663667</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.0714615873774758</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.00243624353471017</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.00451764899230655</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.00617511632619331</v>
+        <v>0.290670709251437</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2013</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.32857950846392</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
+        <v>2010</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>0.137454759567475</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.410167848157459</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.0086399126257143</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.0222308490295306</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.0737313407885046</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.00241746668437432</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.00481728762652694</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.0119610270564952</v>
+        <v>0.252133772699081</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2014</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.334326080980433</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
+        <v>2010</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
       </c>
       <c r="D6" t="n">
-        <v>0.101734914500362</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.431595057885971</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.0236005064249575</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.0794565919426686</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.00249217390808064</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.00496246995360942</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.0218322044039186</v>
+        <v>0.0733053816472367</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2015</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.341673503664889</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
+        <v>2010</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0884855919937461</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.410509175767614</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.00913029512612327</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.0243335861732676</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.0842866430854728</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.00251066184722792</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.00539864859635136</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.0336718937453076</v>
+        <v>0.00230238382452896</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2016</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.330675581183728</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
+        <v>2010</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0705485684728781</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.420809586298719</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.0172990162741022</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.0323968620389084</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.0761357867412523</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.00239561681625303</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.00590618684087012</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.0438327953332886</v>
+        <v>0.0180280502430537</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2017</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.331369893457585</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
+        <v>2010</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0577521051101989</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.403932324957214</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.0312580134749847</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.0353048777013127</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.0795838976402631</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.00233352391553346</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.00616384624005379</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0.052301517502854</v>
+        <v>0.00309929555102816</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2018</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.319154245328742</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
+        <v>2010</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0437033390053524</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.389648517165296</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.0623144717104449</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.0377251652419438</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.0777076213317824</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.00242236483847222</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.00717975885761121</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0.0601445165203554</v>
+        <v>0.00351305981736638</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2019</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.322438841124481</v>
-      </c>
-      <c r="C11" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="n">
         <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.0343351533002472</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.381051176338918</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.0628909173560157</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.0416705698826866</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.0788791475573428</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.00280735730746134</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0.00751093804388234</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0.0684158990889647</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.279514031567449</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.138739425883535</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.378150073272013</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.093966393678015</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.0784135200946303</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.00247102592822759</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0199593518081612</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.00446834621326357</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.00431783155470561</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.309036885418116</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.16871896917671</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.401733664142025</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.0148835897660963</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.0714615873774758</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.00243624353471017</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.0210362952663667</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.00617511632619331</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.00451764899230655</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.32857950846392</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.137454759567475</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.410167848157459</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.0086399126257143</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.0737313407885046</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B46" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.00241746668437432</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.0222308490295306</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B48" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.0119610270564952</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B49" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.00481728762652694</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B50" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B51" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B52" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B53" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.334326080980433</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.101734914500362</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B56" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.431595057885971</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B58" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.0794565919426686</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B59" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.00249217390808064</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B60" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.0236005064249575</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B61" t="s">
+        <v>21</v>
+      </c>
+      <c r="C61" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.0218322044039186</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B62" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.00496246995360942</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B63" t="s">
+        <v>23</v>
+      </c>
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B65" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65" t="s">
+        <v>10</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B66" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B67" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.341673503664889</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B68" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.0884855919937461</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B69" t="s">
+        <v>13</v>
+      </c>
+      <c r="C69" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.410509175767614</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.00913029512612327</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B71" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.0842866430854728</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B72" t="s">
+        <v>20</v>
+      </c>
+      <c r="C72" t="s">
+        <v>10</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.00251066184722792</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B73" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" t="s">
+        <v>10</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.0243335861732676</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B74" t="s">
+        <v>21</v>
+      </c>
+      <c r="C74" t="s">
+        <v>10</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.0336718937453076</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B75" t="s">
+        <v>22</v>
+      </c>
+      <c r="C75" t="s">
+        <v>10</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.00539864859635136</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B76" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76" t="s">
+        <v>10</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B77" t="s">
+        <v>24</v>
+      </c>
+      <c r="C77" t="s">
+        <v>10</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B78" t="s">
+        <v>25</v>
+      </c>
+      <c r="C78" t="s">
+        <v>10</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B79" t="s">
+        <v>26</v>
+      </c>
+      <c r="C79" t="s">
+        <v>10</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B80" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80" t="s">
+        <v>10</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.330675581183728</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B81" t="s">
+        <v>12</v>
+      </c>
+      <c r="C81" t="s">
+        <v>10</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0705485684728781</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B82" t="s">
+        <v>13</v>
+      </c>
+      <c r="C82" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.420809586298719</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B83" t="s">
+        <v>18</v>
+      </c>
+      <c r="C83" t="s">
+        <v>10</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.0172990162741022</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B84" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.0761357867412523</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B85" t="s">
+        <v>20</v>
+      </c>
+      <c r="C85" t="s">
+        <v>10</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0.00239561681625303</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B86" t="s">
+        <v>14</v>
+      </c>
+      <c r="C86" t="s">
+        <v>10</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0.0323968620389084</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B87" t="s">
+        <v>21</v>
+      </c>
+      <c r="C87" t="s">
+        <v>10</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.0438327953332886</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B88" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" t="s">
+        <v>10</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.00590618684087012</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B89" t="s">
+        <v>23</v>
+      </c>
+      <c r="C89" t="s">
+        <v>10</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B90" t="s">
+        <v>24</v>
+      </c>
+      <c r="C90" t="s">
+        <v>10</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B91" t="s">
+        <v>25</v>
+      </c>
+      <c r="C91" t="s">
+        <v>10</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B92" t="s">
+        <v>26</v>
+      </c>
+      <c r="C92" t="s">
+        <v>10</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B93" t="s">
+        <v>11</v>
+      </c>
+      <c r="C93" t="s">
+        <v>10</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.331369893457585</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B94" t="s">
+        <v>12</v>
+      </c>
+      <c r="C94" t="s">
+        <v>10</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.0577521051101989</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B95" t="s">
+        <v>13</v>
+      </c>
+      <c r="C95" t="s">
+        <v>10</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.403932324957214</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B96" t="s">
+        <v>18</v>
+      </c>
+      <c r="C96" t="s">
+        <v>10</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0.0312580134749847</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B97" t="s">
+        <v>19</v>
+      </c>
+      <c r="C97" t="s">
+        <v>10</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0.0795838976402631</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B98" t="s">
+        <v>20</v>
+      </c>
+      <c r="C98" t="s">
+        <v>10</v>
+      </c>
+      <c r="D98" t="n">
+        <v>0.00233352391553346</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B99" t="s">
+        <v>14</v>
+      </c>
+      <c r="C99" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0.0353048777013127</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B100" t="s">
+        <v>21</v>
+      </c>
+      <c r="C100" t="s">
+        <v>10</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0.052301517502854</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B101" t="s">
+        <v>22</v>
+      </c>
+      <c r="C101" t="s">
+        <v>10</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0.00616384624005379</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B102" t="s">
+        <v>23</v>
+      </c>
+      <c r="C102" t="s">
+        <v>10</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B103" t="s">
+        <v>24</v>
+      </c>
+      <c r="C103" t="s">
+        <v>10</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B104" t="s">
+        <v>25</v>
+      </c>
+      <c r="C104" t="s">
+        <v>10</v>
+      </c>
+      <c r="D104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B105" t="s">
+        <v>26</v>
+      </c>
+      <c r="C105" t="s">
+        <v>10</v>
+      </c>
+      <c r="D105" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B106" t="s">
+        <v>11</v>
+      </c>
+      <c r="C106" t="s">
+        <v>10</v>
+      </c>
+      <c r="D106" t="n">
+        <v>0.319154245328742</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B107" t="s">
+        <v>12</v>
+      </c>
+      <c r="C107" t="s">
+        <v>10</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0.0437033390053524</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B108" t="s">
+        <v>13</v>
+      </c>
+      <c r="C108" t="s">
+        <v>10</v>
+      </c>
+      <c r="D108" t="n">
+        <v>0.389648517165296</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B109" t="s">
+        <v>18</v>
+      </c>
+      <c r="C109" t="s">
+        <v>10</v>
+      </c>
+      <c r="D109" t="n">
+        <v>0.0623144717104449</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B110" t="s">
+        <v>19</v>
+      </c>
+      <c r="C110" t="s">
+        <v>10</v>
+      </c>
+      <c r="D110" t="n">
+        <v>0.0777076213317824</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B111" t="s">
+        <v>20</v>
+      </c>
+      <c r="C111" t="s">
+        <v>10</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0.00242236483847222</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B112" t="s">
+        <v>14</v>
+      </c>
+      <c r="C112" t="s">
+        <v>10</v>
+      </c>
+      <c r="D112" t="n">
+        <v>0.0377251652419438</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B113" t="s">
+        <v>21</v>
+      </c>
+      <c r="C113" t="s">
+        <v>10</v>
+      </c>
+      <c r="D113" t="n">
+        <v>0.0601445165203554</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B114" t="s">
+        <v>22</v>
+      </c>
+      <c r="C114" t="s">
+        <v>10</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0.00717975885761121</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B115" t="s">
+        <v>23</v>
+      </c>
+      <c r="C115" t="s">
+        <v>10</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B116" t="s">
+        <v>24</v>
+      </c>
+      <c r="C116" t="s">
+        <v>10</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B117" t="s">
+        <v>25</v>
+      </c>
+      <c r="C117" t="s">
+        <v>10</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B118" t="s">
+        <v>26</v>
+      </c>
+      <c r="C118" t="s">
+        <v>10</v>
+      </c>
+      <c r="D118" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B119" t="s">
+        <v>11</v>
+      </c>
+      <c r="C119" t="s">
+        <v>10</v>
+      </c>
+      <c r="D119" t="n">
+        <v>0.322438841124481</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B120" t="s">
+        <v>12</v>
+      </c>
+      <c r="C120" t="s">
+        <v>10</v>
+      </c>
+      <c r="D120" t="n">
+        <v>0.0343351533002472</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B121" t="s">
+        <v>13</v>
+      </c>
+      <c r="C121" t="s">
+        <v>10</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0.381051176338918</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B122" t="s">
+        <v>18</v>
+      </c>
+      <c r="C122" t="s">
+        <v>10</v>
+      </c>
+      <c r="D122" t="n">
+        <v>0.0628909173560157</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B123" t="s">
+        <v>19</v>
+      </c>
+      <c r="C123" t="s">
+        <v>10</v>
+      </c>
+      <c r="D123" t="n">
+        <v>0.0788791475573428</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B124" t="s">
+        <v>20</v>
+      </c>
+      <c r="C124" t="s">
+        <v>10</v>
+      </c>
+      <c r="D124" t="n">
+        <v>0.00280735730746134</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B125" t="s">
+        <v>14</v>
+      </c>
+      <c r="C125" t="s">
+        <v>10</v>
+      </c>
+      <c r="D125" t="n">
+        <v>0.0416705698826866</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B126" t="s">
+        <v>21</v>
+      </c>
+      <c r="C126" t="s">
+        <v>10</v>
+      </c>
+      <c r="D126" t="n">
+        <v>0.0684158990889647</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B127" t="s">
+        <v>22</v>
+      </c>
+      <c r="C127" t="s">
+        <v>10</v>
+      </c>
+      <c r="D127" t="n">
+        <v>0.00751093804388234</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B128" t="s">
+        <v>23</v>
+      </c>
+      <c r="C128" t="s">
+        <v>10</v>
+      </c>
+      <c r="D128" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B129" t="s">
+        <v>24</v>
+      </c>
+      <c r="C129" t="s">
+        <v>10</v>
+      </c>
+      <c r="D129" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B130" t="s">
+        <v>25</v>
+      </c>
+      <c r="C130" t="s">
+        <v>10</v>
+      </c>
+      <c r="D130" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B131" t="s">
+        <v>26</v>
+      </c>
+      <c r="C131" t="s">
+        <v>10</v>
+      </c>
+      <c r="D131" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
         <v>2020</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B132" t="s">
+        <v>11</v>
+      </c>
+      <c r="C132" t="s">
+        <v>10</v>
+      </c>
+      <c r="D132" t="n">
         <v>0.313426983789406</v>
       </c>
-      <c r="C12" t="n">
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B133" t="s">
+        <v>12</v>
+      </c>
+      <c r="C133" t="s">
+        <v>10</v>
+      </c>
+      <c r="D133" t="n">
+        <v>0.0321379578663662</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B134" t="s">
+        <v>13</v>
+      </c>
+      <c r="C134" t="s">
+        <v>10</v>
+      </c>
+      <c r="D134" t="n">
+        <v>0.397941195147002</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B135" t="s">
+        <v>18</v>
+      </c>
+      <c r="C135" t="s">
+        <v>10</v>
+      </c>
+      <c r="D135" t="n">
+        <v>0.0390594368272674</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B136" t="s">
+        <v>19</v>
+      </c>
+      <c r="C136" t="s">
+        <v>10</v>
+      </c>
+      <c r="D136" t="n">
+        <v>0.0794322109322477</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B137" t="s">
+        <v>20</v>
+      </c>
+      <c r="C137" t="s">
+        <v>10</v>
+      </c>
+      <c r="D137" t="n">
+        <v>0.00301573686486334</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B138" t="s">
+        <v>14</v>
+      </c>
+      <c r="C138" t="s">
+        <v>10</v>
+      </c>
+      <c r="D138" t="n">
+        <v>0.0462308832823151</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B139" t="s">
+        <v>21</v>
+      </c>
+      <c r="C139" t="s">
+        <v>10</v>
+      </c>
+      <c r="D139" t="n">
+        <v>0.0797144322966066</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B140" t="s">
+        <v>22</v>
+      </c>
+      <c r="C140" t="s">
+        <v>10</v>
+      </c>
+      <c r="D140" t="n">
+        <v>0.00904116299392519</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B141" t="s">
+        <v>23</v>
+      </c>
+      <c r="C141" t="s">
+        <v>10</v>
+      </c>
+      <c r="D141" t="n">
         <v>0</v>
       </c>
-      <c r="D12" t="n">
-        <v>0.0321379578663662</v>
-      </c>
-      <c r="E12" t="n">
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B142" t="s">
+        <v>24</v>
+      </c>
+      <c r="C142" t="s">
+        <v>10</v>
+      </c>
+      <c r="D142" t="n">
         <v>0</v>
       </c>
-      <c r="F12" t="n">
-        <v>0.397941195147002</v>
-      </c>
-      <c r="G12" t="n">
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B143" t="s">
+        <v>25</v>
+      </c>
+      <c r="C143" t="s">
+        <v>10</v>
+      </c>
+      <c r="D143" t="n">
         <v>0</v>
       </c>
-      <c r="H12" t="n">
-        <v>0.0390594368272674</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0.0462308832823151</v>
-      </c>
-      <c r="J12" t="n">
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B144" t="s">
+        <v>26</v>
+      </c>
+      <c r="C144" t="s">
+        <v>10</v>
+      </c>
+      <c r="D144" t="n">
         <v>0</v>
       </c>
-      <c r="K12" t="n">
-        <v>0.0794322109322477</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.00301573686486334</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0.00904116299392519</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.0797144322966066</v>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B145" t="s">
+        <v>11</v>
+      </c>
+      <c r="C145" t="s">
+        <v>11</v>
+      </c>
+      <c r="D145" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B146" t="s">
+        <v>12</v>
+      </c>
+      <c r="C146" t="s">
+        <v>12</v>
+      </c>
+      <c r="D146" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B147" t="s">
+        <v>13</v>
+      </c>
+      <c r="C147" t="s">
+        <v>13</v>
+      </c>
+      <c r="D147" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B148" t="s">
+        <v>14</v>
+      </c>
+      <c r="C148" t="s">
+        <v>14</v>
+      </c>
+      <c r="D148" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B149" t="s">
+        <v>11</v>
+      </c>
+      <c r="C149" t="s">
+        <v>11</v>
+      </c>
+      <c r="D149" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B150" t="s">
+        <v>12</v>
+      </c>
+      <c r="C150" t="s">
+        <v>12</v>
+      </c>
+      <c r="D150" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B151" t="s">
+        <v>13</v>
+      </c>
+      <c r="C151" t="s">
+        <v>13</v>
+      </c>
+      <c r="D151" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B152" t="s">
+        <v>14</v>
+      </c>
+      <c r="C152" t="s">
+        <v>14</v>
+      </c>
+      <c r="D152" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B153" t="s">
+        <v>11</v>
+      </c>
+      <c r="C153" t="s">
+        <v>11</v>
+      </c>
+      <c r="D153" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B154" t="s">
+        <v>12</v>
+      </c>
+      <c r="C154" t="s">
+        <v>12</v>
+      </c>
+      <c r="D154" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B155" t="s">
+        <v>13</v>
+      </c>
+      <c r="C155" t="s">
+        <v>13</v>
+      </c>
+      <c r="D155" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B156" t="s">
+        <v>14</v>
+      </c>
+      <c r="C156" t="s">
+        <v>14</v>
+      </c>
+      <c r="D156" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B157" t="s">
+        <v>11</v>
+      </c>
+      <c r="C157" t="s">
+        <v>11</v>
+      </c>
+      <c r="D157" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B158" t="s">
+        <v>12</v>
+      </c>
+      <c r="C158" t="s">
+        <v>12</v>
+      </c>
+      <c r="D158" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B159" t="s">
+        <v>13</v>
+      </c>
+      <c r="C159" t="s">
+        <v>13</v>
+      </c>
+      <c r="D159" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B160" t="s">
+        <v>14</v>
+      </c>
+      <c r="C160" t="s">
+        <v>14</v>
+      </c>
+      <c r="D160" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B161" t="s">
+        <v>11</v>
+      </c>
+      <c r="C161" t="s">
+        <v>11</v>
+      </c>
+      <c r="D161" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B162" t="s">
+        <v>12</v>
+      </c>
+      <c r="C162" t="s">
+        <v>12</v>
+      </c>
+      <c r="D162" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B163" t="s">
+        <v>13</v>
+      </c>
+      <c r="C163" t="s">
+        <v>13</v>
+      </c>
+      <c r="D163" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B164" t="s">
+        <v>14</v>
+      </c>
+      <c r="C164" t="s">
+        <v>14</v>
+      </c>
+      <c r="D164" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B165" t="s">
+        <v>11</v>
+      </c>
+      <c r="C165" t="s">
+        <v>11</v>
+      </c>
+      <c r="D165" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B166" t="s">
+        <v>12</v>
+      </c>
+      <c r="C166" t="s">
+        <v>12</v>
+      </c>
+      <c r="D166" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B167" t="s">
+        <v>13</v>
+      </c>
+      <c r="C167" t="s">
+        <v>13</v>
+      </c>
+      <c r="D167" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B168" t="s">
+        <v>14</v>
+      </c>
+      <c r="C168" t="s">
+        <v>14</v>
+      </c>
+      <c r="D168" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B169" t="s">
+        <v>11</v>
+      </c>
+      <c r="C169" t="s">
+        <v>11</v>
+      </c>
+      <c r="D169" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B170" t="s">
+        <v>12</v>
+      </c>
+      <c r="C170" t="s">
+        <v>12</v>
+      </c>
+      <c r="D170" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B171" t="s">
+        <v>13</v>
+      </c>
+      <c r="C171" t="s">
+        <v>13</v>
+      </c>
+      <c r="D171" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B172" t="s">
+        <v>14</v>
+      </c>
+      <c r="C172" t="s">
+        <v>14</v>
+      </c>
+      <c r="D172" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B173" t="s">
+        <v>11</v>
+      </c>
+      <c r="C173" t="s">
+        <v>11</v>
+      </c>
+      <c r="D173" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B174" t="s">
+        <v>12</v>
+      </c>
+      <c r="C174" t="s">
+        <v>12</v>
+      </c>
+      <c r="D174" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B175" t="s">
+        <v>13</v>
+      </c>
+      <c r="C175" t="s">
+        <v>13</v>
+      </c>
+      <c r="D175" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B176" t="s">
+        <v>14</v>
+      </c>
+      <c r="C176" t="s">
+        <v>14</v>
+      </c>
+      <c r="D176" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B177" t="s">
+        <v>11</v>
+      </c>
+      <c r="C177" t="s">
+        <v>11</v>
+      </c>
+      <c r="D177" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B178" t="s">
+        <v>12</v>
+      </c>
+      <c r="C178" t="s">
+        <v>12</v>
+      </c>
+      <c r="D178" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B179" t="s">
+        <v>13</v>
+      </c>
+      <c r="C179" t="s">
+        <v>13</v>
+      </c>
+      <c r="D179" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B180" t="s">
+        <v>14</v>
+      </c>
+      <c r="C180" t="s">
+        <v>14</v>
+      </c>
+      <c r="D180" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B181" t="s">
+        <v>11</v>
+      </c>
+      <c r="C181" t="s">
+        <v>11</v>
+      </c>
+      <c r="D181" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B182" t="s">
+        <v>12</v>
+      </c>
+      <c r="C182" t="s">
+        <v>12</v>
+      </c>
+      <c r="D182" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B183" t="s">
+        <v>13</v>
+      </c>
+      <c r="C183" t="s">
+        <v>13</v>
+      </c>
+      <c r="D183" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B184" t="s">
+        <v>14</v>
+      </c>
+      <c r="C184" t="s">
+        <v>14</v>
+      </c>
+      <c r="D184" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B185" t="s">
+        <v>11</v>
+      </c>
+      <c r="C185" t="s">
+        <v>11</v>
+      </c>
+      <c r="D185" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B186" t="s">
+        <v>12</v>
+      </c>
+      <c r="C186" t="s">
+        <v>12</v>
+      </c>
+      <c r="D186" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B187" t="s">
+        <v>13</v>
+      </c>
+      <c r="C187" t="s">
+        <v>13</v>
+      </c>
+      <c r="D187" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B188" t="s">
+        <v>14</v>
+      </c>
+      <c r="C188" t="s">
+        <v>14</v>
+      </c>
+      <c r="D188" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2206,19 +4324,19 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
@@ -2227,19 +4345,19 @@
         <v>14</v>
       </c>
       <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>20</v>
-      </c>
-      <c r="L1" t="s">
-        <v>21</v>
       </c>
       <c r="M1" t="s">
         <v>22</v>
       </c>
       <c r="N1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
@@ -2277,7 +4395,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
         <v>1</v>
@@ -2321,7 +4439,7 @@
         <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
         <v>1</v>
@@ -2365,7 +4483,7 @@
         <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
         <v>1</v>
@@ -2409,7 +4527,7 @@
         <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M5" t="n">
         <v>1</v>
@@ -2453,7 +4571,7 @@
         <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M6" t="n">
         <v>1</v>
@@ -2497,7 +4615,7 @@
         <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
         <v>1</v>
@@ -2541,7 +4659,7 @@
         <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M8" t="n">
         <v>1</v>
@@ -2585,7 +4703,7 @@
         <v>1</v>
       </c>
       <c r="L9" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M9" t="n">
         <v>1</v>
@@ -2629,7 +4747,7 @@
         <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M10" t="n">
         <v>1</v>
@@ -2673,7 +4791,7 @@
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M11" t="n">
         <v>1</v>
@@ -2717,7 +4835,7 @@
         <v>1</v>
       </c>
       <c r="L12" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M12" t="n">
         <v>1</v>
@@ -2761,7 +4879,7 @@
         <v>1</v>
       </c>
       <c r="L13" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M13" t="n">
         <v>1</v>
@@ -2805,7 +4923,7 @@
         <v>1</v>
       </c>
       <c r="L14" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M14" t="n">
         <v>1</v>
@@ -2849,7 +4967,7 @@
         <v>1</v>
       </c>
       <c r="L15" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M15" t="n">
         <v>1</v>
@@ -2893,7 +5011,7 @@
         <v>1</v>
       </c>
       <c r="L16" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M16" t="n">
         <v>1</v>
@@ -2937,7 +5055,7 @@
         <v>1</v>
       </c>
       <c r="L17" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M17" t="n">
         <v>1</v>
@@ -2981,7 +5099,7 @@
         <v>1</v>
       </c>
       <c r="L18" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M18" t="n">
         <v>1</v>
@@ -3025,7 +5143,7 @@
         <v>1</v>
       </c>
       <c r="L19" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M19" t="n">
         <v>1</v>
@@ -3069,7 +5187,7 @@
         <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M20" t="n">
         <v>1</v>
@@ -3113,7 +5231,7 @@
         <v>1</v>
       </c>
       <c r="L21" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M21" t="n">
         <v>1</v>
@@ -3157,7 +5275,7 @@
         <v>1</v>
       </c>
       <c r="L22" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M22" t="n">
         <v>1</v>
@@ -3201,7 +5319,7 @@
         <v>1</v>
       </c>
       <c r="L23" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M23" t="n">
         <v>1</v>
@@ -3245,7 +5363,7 @@
         <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M24" t="n">
         <v>1</v>
@@ -3289,7 +5407,7 @@
         <v>1</v>
       </c>
       <c r="L25" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M25" t="n">
         <v>1</v>
@@ -3333,7 +5451,7 @@
         <v>1</v>
       </c>
       <c r="L26" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M26" t="n">
         <v>1</v>
@@ -3377,7 +5495,7 @@
         <v>1</v>
       </c>
       <c r="L27" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M27" t="n">
         <v>1</v>
@@ -3421,7 +5539,7 @@
         <v>1</v>
       </c>
       <c r="L28" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M28" t="n">
         <v>1</v>
@@ -3465,7 +5583,7 @@
         <v>1</v>
       </c>
       <c r="L29" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M29" t="n">
         <v>1</v>
@@ -3509,7 +5627,7 @@
         <v>1</v>
       </c>
       <c r="L30" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M30" t="n">
         <v>1</v>
@@ -3553,7 +5671,7 @@
         <v>1</v>
       </c>
       <c r="L31" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M31" t="n">
         <v>1</v>
@@ -3597,7 +5715,7 @@
         <v>1</v>
       </c>
       <c r="L32" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M32" t="n">
         <v>1</v>
@@ -3641,7 +5759,7 @@
         <v>1</v>
       </c>
       <c r="L33" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M33" t="n">
         <v>1</v>
@@ -3685,7 +5803,7 @@
         <v>1</v>
       </c>
       <c r="L34" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M34" t="n">
         <v>1</v>
@@ -3729,7 +5847,7 @@
         <v>1</v>
       </c>
       <c r="L35" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M35" t="n">
         <v>1</v>
@@ -3773,7 +5891,7 @@
         <v>1</v>
       </c>
       <c r="L36" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M36" t="n">
         <v>1</v>
@@ -3817,7 +5935,7 @@
         <v>1</v>
       </c>
       <c r="L37" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M37" t="n">
         <v>1</v>
@@ -3861,7 +5979,7 @@
         <v>1</v>
       </c>
       <c r="L38" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M38" t="n">
         <v>1</v>
@@ -3905,7 +6023,7 @@
         <v>1</v>
       </c>
       <c r="L39" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M39" t="n">
         <v>1</v>
@@ -3949,7 +6067,7 @@
         <v>1</v>
       </c>
       <c r="L40" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M40" t="n">
         <v>1</v>
@@ -3993,7 +6111,7 @@
         <v>1</v>
       </c>
       <c r="L41" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M41" t="n">
         <v>1</v>
@@ -4037,7 +6155,7 @@
         <v>1</v>
       </c>
       <c r="L42" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M42" t="n">
         <v>1</v>
@@ -4065,19 +6183,19 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
         <v>18</v>
@@ -4086,19 +6204,19 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>21</v>
       </c>
       <c r="L1" t="s">
         <v>22</v>
       </c>
       <c r="M1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
@@ -4124,10 +6242,10 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
         <v>-95</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -4373,7 +6491,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
@@ -5170,6 +7288,206 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="n">
+        <v>8.58534635183259</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="n">
+        <v>13.1853861045125</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="n">
+        <v>21.1087169869477</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="n">
+        <v>24.9631016042781</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="n">
+        <v>8.49987390942158</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="n">
+        <v>11.2693464104693</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="n">
+        <v>9.64032450223761</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="n">
+        <v>28.1380168996814</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="n">
+        <v>33.0910873440285</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="n">
+        <v>8.6716549684072</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="n">
+        <v>10.9084249470451</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="n">
+        <v>11.7867578322641</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="n">
+        <v>10.4950947817005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2082.78711805897</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2082.78711805897</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3464.72222222222</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5942.47222222222</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5942.47222222222</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2255.74973508559</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2255.74973508559</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3255.55555555556</v>
+      </c>
+      <c r="E3" t="n">
+        <v>7568.65833333333</v>
+      </c>
+      <c r="F3" t="n">
+        <v>7568.65833333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>

</xml_diff>